<commit_message>
Added comments and reformatted the xlsx file to be cleaner. TODO Gather info from group and populate the xlsx file.
</commit_message>
<xml_diff>
--- a/src/GradDataWarehousing/HW4/HW4.xlsx
+++ b/src/GradDataWarehousing/HW4/HW4.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Combine Sales (December)</t>
   </si>
@@ -36,12 +36,6 @@
     <t>Sam's Market</t>
   </si>
   <si>
-    <t>Combined Customer Count</t>
-  </si>
-  <si>
-    <t>Combined Sales (USD)</t>
-  </si>
-  <si>
     <t>Best Sellting Items Combined</t>
   </si>
   <si>
@@ -112,14 +106,37 @@
   </si>
   <si>
     <t>Rank</t>
+  </si>
+  <si>
+    <t>Total Combined</t>
+  </si>
+  <si>
+    <t>Sales (USD)</t>
+  </si>
+  <si>
+    <t>Customer Count</t>
+  </si>
+  <si>
+    <t>Units Sold</t>
+  </si>
+  <si>
+    <t>SKU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -135,7 +152,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -143,14 +160,110 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,89 +567,147 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="37.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1">
         <f>D2+F2+H2</f>
         <v>6935692.9199999999</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <v>6935692.9199999999</v>
       </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2">
         <f>D3+F3+H3</f>
         <v>36481</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="6">
         <v>36481</v>
       </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2">
+        <f>D4+F4+H4</f>
+        <v>1847171</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1847171</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -544,450 +715,550 @@
         <v>42355001</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <f>D8+F8+H8</f>
         <v>5075</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="7">
         <v>5075</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="5">
         <v>5</v>
       </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>42359001</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <f t="shared" ref="C9:C32" si="0">D9+F9+H9</f>
         <v>5105</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="7">
         <v>5105</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="5">
         <v>3</v>
       </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>42357001</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
         <v>5068</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="7">
         <v>5068</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <v>6</v>
       </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>42360001</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
         <v>5201</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="7">
         <v>5201</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <v>1</v>
       </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>42356001</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
         <v>5104</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="7">
         <v>5104</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="5">
         <v>4</v>
       </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>42358001</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
         <v>5107</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="7">
         <v>5107</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <v>2</v>
       </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>42314001</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
         <v>2026</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="7">
         <v>2026</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="5">
         <v>9</v>
       </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>42312001</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
         <v>2029</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="7">
         <v>2029</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="5">
         <v>8</v>
       </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>42311001</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
         <v>2006</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="7">
         <v>2006</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="7"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>42313001</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
         <v>2087</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="7">
         <v>2087</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="7"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>42671001</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
         <v>1249</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="7">
         <v>1249</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="7"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>42526001</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
         <v>1158</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="7">
         <v>1158</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="5">
         <v>58</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="7"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>42349001</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
         <v>1218</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="7">
         <v>1218</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="5">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="7"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>42576001</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
         <v>1236</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="7">
         <v>1236</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="5">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="7"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>42572001</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="7">
         <v>1200</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="5">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="7"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>42583001</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
         <v>1179</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="7">
         <v>1179</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="5">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="7"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>42584001</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
         <v>1191</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="7">
         <v>1191</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="5">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="7"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>42528001</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
         <v>1279</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="7">
         <v>1279</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="5">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="7"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>43526001</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
         <v>1185</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="7">
         <v>1185</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="5">
         <v>46</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="7"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>42334001</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
         <v>1199</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="7">
         <v>1199</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="5">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="7"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>42266001</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
         <v>1194</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="7">
         <v>1194</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="7"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>42573001</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
         <v>1212</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="7">
         <v>1212</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="5">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="7"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>42581001</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
         <v>1206</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="7">
         <v>1206</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="5">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="7"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>42574001</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
         <v>1236</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="7">
         <v>1236</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="5">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="7"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>42527001</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
         <v>1188</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="8">
         <v>1188</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="9">
         <v>43</v>
       </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>